<commit_message>
calc data: fix typos
</commit_message>
<xml_diff>
--- a/public/local/fixtures/calculator/Технадзор контроль калькуляторы.xlsx
+++ b/public/local/fixtures/calculator/Технадзор контроль калькуляторы.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="960" yWindow="460" windowWidth="37480" windowHeight="23540" activeTab="1"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="37480" windowHeight="23540"/>
   </bookViews>
   <sheets>
     <sheet name="Технадзор одного здания" sheetId="3" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Московская область</t>
   </si>
   <si>
-    <t>Санкт-Петерьборг</t>
-  </si>
-  <si>
     <t>Ленинградская область</t>
   </si>
   <si>
@@ -595,6 +592,9 @@
   </si>
   <si>
     <t>Расстояние между объектами 0,5-3 км</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург</t>
   </si>
 </sst>
 </file>
@@ -1696,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF237"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B205" sqref="B205"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="4" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" s="15"/>
     </row>
@@ -1738,7 +1738,7 @@
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" s="15"/>
     </row>
@@ -1764,7 +1764,7 @@
     <row r="9" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="30"/>
       <c r="B9" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" s="15"/>
       <c r="AD9" s="13"/>
@@ -1804,7 +1804,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>4</v>
+        <v>189</v>
       </c>
       <c r="C12" s="15">
         <v>2</v>
@@ -1818,7 +1818,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="15">
         <v>2</v>
@@ -1832,7 +1832,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="15">
         <v>2.2000000000000002</v>
@@ -1846,7 +1846,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="15">
         <v>2.5</v>
@@ -1860,7 +1860,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="15">
         <v>3</v>
@@ -1874,7 +1874,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="15">
         <v>2</v>
@@ -1888,7 +1888,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="15">
         <v>2</v>
@@ -1902,7 +1902,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="15">
         <v>2</v>
@@ -1916,7 +1916,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="15">
         <v>2</v>
@@ -1930,7 +1930,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="15">
         <v>1.8</v>
@@ -1944,7 +1944,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="15">
         <v>2.5</v>
@@ -1958,7 +1958,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="15">
         <v>1.2</v>
@@ -1972,7 +1972,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="15">
         <v>2.2000000000000002</v>
@@ -1986,7 +1986,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" s="15">
         <v>1.5</v>
@@ -2000,7 +2000,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" s="15">
         <v>1.8</v>
@@ -2014,7 +2014,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="15">
         <v>2</v>
@@ -2028,7 +2028,7 @@
         <v>19</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28" s="15">
         <v>3</v>
@@ -2042,7 +2042,7 @@
         <v>20</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29" s="15">
         <v>3</v>
@@ -2056,7 +2056,7 @@
         <v>21</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30" s="15">
         <v>1.5</v>
@@ -2070,7 +2070,7 @@
         <v>22</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" s="15">
         <v>2</v>
@@ -2084,7 +2084,7 @@
         <v>23</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="15">
         <v>2.5</v>
@@ -2098,7 +2098,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="15">
         <v>2</v>
@@ -2112,7 +2112,7 @@
         <v>25</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="15">
         <v>2</v>
@@ -2126,7 +2126,7 @@
         <v>26</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C35" s="15">
         <v>2</v>
@@ -2140,7 +2140,7 @@
         <v>27</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="15">
         <v>1.5</v>
@@ -2154,7 +2154,7 @@
         <v>28</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="15">
         <v>3</v>
@@ -2168,7 +2168,7 @@
         <v>29</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" s="15">
         <v>2</v>
@@ -2182,7 +2182,7 @@
         <v>30</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="15">
         <v>2</v>
@@ -2196,7 +2196,7 @@
         <v>31</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="15">
         <v>2.5</v>
@@ -2210,7 +2210,7 @@
         <v>32</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41" s="15">
         <v>2</v>
@@ -2224,7 +2224,7 @@
         <v>33</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42" s="15">
         <v>2.5</v>
@@ -2238,7 +2238,7 @@
         <v>34</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" s="15">
         <v>2</v>
@@ -2252,7 +2252,7 @@
         <v>35</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C44" s="15">
         <v>2</v>
@@ -2266,7 +2266,7 @@
         <v>36</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C45" s="15">
         <v>2.5</v>
@@ -2280,7 +2280,7 @@
         <v>37</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" s="15">
         <v>2.2000000000000002</v>
@@ -2294,7 +2294,7 @@
         <v>38</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C47" s="15">
         <v>2.5</v>
@@ -2308,7 +2308,7 @@
         <v>39</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C48" s="15">
         <v>2</v>
@@ -2322,7 +2322,7 @@
         <v>40</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C49" s="15">
         <v>2</v>
@@ -2336,7 +2336,7 @@
         <v>41</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C50" s="15">
         <v>3</v>
@@ -2350,7 +2350,7 @@
         <v>42</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C51" s="15">
         <v>3</v>
@@ -2364,7 +2364,7 @@
         <v>43</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C52" s="15">
         <v>2</v>
@@ -2378,7 +2378,7 @@
         <v>44</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C53" s="15">
         <v>2.5</v>
@@ -2392,7 +2392,7 @@
         <v>45</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C54" s="15">
         <v>2.5</v>
@@ -2406,7 +2406,7 @@
         <v>46</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C55" s="15">
         <v>2</v>
@@ -2420,7 +2420,7 @@
         <v>47</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C56" s="15">
         <v>2</v>
@@ -2434,7 +2434,7 @@
         <v>48</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C57" s="15">
         <v>2.5</v>
@@ -2448,7 +2448,7 @@
         <v>49</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C58" s="15">
         <v>2.2999999999999998</v>
@@ -2462,7 +2462,7 @@
         <v>50</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C59" s="15">
         <v>2.2999999999999998</v>
@@ -2476,7 +2476,7 @@
         <v>51</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C60" s="15">
         <v>1.8</v>
@@ -2490,7 +2490,7 @@
         <v>52</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C61" s="15">
         <v>2</v>
@@ -2504,7 +2504,7 @@
         <v>53</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C62" s="15">
         <v>2.5</v>
@@ -2518,7 +2518,7 @@
         <v>54</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C63" s="15">
         <v>3</v>
@@ -2532,7 +2532,7 @@
         <v>55</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C64" s="15">
         <v>2</v>
@@ -2546,7 +2546,7 @@
         <v>56</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C65" s="15">
         <v>2.5</v>
@@ -2560,7 +2560,7 @@
         <v>57</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C66" s="15">
         <v>2</v>
@@ -2574,7 +2574,7 @@
         <v>58</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C67" s="15">
         <v>1.5</v>
@@ -2588,7 +2588,7 @@
         <v>59</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C68" s="15">
         <v>2</v>
@@ -2602,7 +2602,7 @@
         <v>60</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C69" s="15">
         <v>2</v>
@@ -2616,7 +2616,7 @@
         <v>61</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C70" s="15">
         <v>3</v>
@@ -2630,7 +2630,7 @@
         <v>62</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C71" s="15">
         <v>2.8</v>
@@ -2644,7 +2644,7 @@
         <v>63</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C72" s="15">
         <v>2.5</v>
@@ -2658,7 +2658,7 @@
         <v>64</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C73" s="15">
         <v>2</v>
@@ -2672,7 +2672,7 @@
         <v>65</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C74" s="15">
         <v>1.8</v>
@@ -2686,7 +2686,7 @@
         <v>66</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C75" s="15">
         <v>2</v>
@@ -2700,7 +2700,7 @@
         <v>67</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C76" s="15">
         <v>1.8</v>
@@ -2714,7 +2714,7 @@
         <v>68</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C77" s="15">
         <v>2.2000000000000002</v>
@@ -2728,7 +2728,7 @@
         <v>69</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C78" s="15">
         <v>1.5</v>
@@ -2742,7 +2742,7 @@
         <v>70</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C79" s="15">
         <v>2.5</v>
@@ -2756,7 +2756,7 @@
         <v>71</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C80" s="15">
         <v>1.8</v>
@@ -2770,7 +2770,7 @@
         <v>72</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C81" s="15">
         <v>2.5</v>
@@ -2784,7 +2784,7 @@
         <v>73</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C82" s="15">
         <v>2.2000000000000002</v>
@@ -2798,7 +2798,7 @@
         <v>74</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C83" s="15">
         <v>2.5</v>
@@ -2812,7 +2812,7 @@
         <v>75</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C84" s="15">
         <v>2.2000000000000002</v>
@@ -2826,7 +2826,7 @@
         <v>76</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C85" s="15">
         <v>3</v>
@@ -2840,7 +2840,7 @@
         <v>77</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C86" s="15">
         <v>2.8</v>
@@ -2854,7 +2854,7 @@
         <v>78</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C87" s="15">
         <v>2.5</v>
@@ -2868,7 +2868,7 @@
         <v>79</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C88" s="15">
         <v>2.2000000000000002</v>
@@ -2882,7 +2882,7 @@
         <v>80</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C89" s="15">
         <v>2</v>
@@ -2896,7 +2896,7 @@
         <v>81</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C90" s="15">
         <v>2</v>
@@ -2910,7 +2910,7 @@
         <v>82</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C91" s="15">
         <v>3</v>
@@ -2924,7 +2924,7 @@
         <v>83</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C92" s="15">
         <v>2.8</v>
@@ -2938,7 +2938,7 @@
         <v>84</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C93" s="15">
         <v>1.8</v>
@@ -2976,7 +2976,7 @@
     <row r="97" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="30"/>
       <c r="B97" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C97" s="15"/>
       <c r="AD97" s="13"/>
@@ -2988,7 +2988,7 @@
         <v>1</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C98" s="15">
         <v>1</v>
@@ -3002,7 +3002,7 @@
         <v>2</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C99" s="15">
         <v>0.95</v>
@@ -3016,7 +3016,7 @@
         <v>3</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C100" s="15">
         <v>0.85</v>
@@ -3030,7 +3030,7 @@
         <v>4</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C101" s="15">
         <v>0.9</v>
@@ -3044,7 +3044,7 @@
         <v>5</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C102" s="15">
         <v>0.8</v>
@@ -3058,7 +3058,7 @@
         <v>6</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C103" s="15">
         <v>0.8</v>
@@ -3072,7 +3072,7 @@
         <v>7</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C104" s="15">
         <v>0.8</v>
@@ -3086,7 +3086,7 @@
         <v>8</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C105" s="15">
         <v>1.1000000000000001</v>
@@ -3100,7 +3100,7 @@
         <v>9</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C106" s="15">
         <v>1.1000000000000001</v>
@@ -3114,7 +3114,7 @@
         <v>10</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C107" s="15">
         <v>1.1000000000000001</v>
@@ -3128,7 +3128,7 @@
         <v>11</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C108" s="15">
         <v>1.1000000000000001</v>
@@ -3142,7 +3142,7 @@
         <v>12</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C109" s="15">
         <v>0.8</v>
@@ -3156,7 +3156,7 @@
         <v>13</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C110" s="15">
         <v>1</v>
@@ -3170,7 +3170,7 @@
         <v>14</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C111" s="15">
         <v>1</v>
@@ -3184,7 +3184,7 @@
         <v>15</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C112" s="15">
         <v>1</v>
@@ -3198,7 +3198,7 @@
         <v>16</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C113" s="15">
         <v>0.8</v>
@@ -3212,7 +3212,7 @@
         <v>17</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C114" s="15">
         <v>1</v>
@@ -3226,7 +3226,7 @@
         <v>18</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C115" s="15">
         <v>1</v>
@@ -3240,7 +3240,7 @@
         <v>19</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C116" s="15">
         <v>1</v>
@@ -3260,7 +3260,7 @@
     <row r="118" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="30"/>
       <c r="B118" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C118" s="15"/>
       <c r="AD118" s="13"/>
@@ -3272,7 +3272,7 @@
         <v>1</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C119" s="15">
         <v>1</v>
@@ -3286,7 +3286,7 @@
         <v>2</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C120" s="15">
         <v>1</v>
@@ -3300,7 +3300,7 @@
         <v>3</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C121" s="15">
         <v>1</v>
@@ -3314,7 +3314,7 @@
         <v>4</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C122" s="15">
         <v>0.9</v>
@@ -3334,7 +3334,7 @@
     <row r="124" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="30"/>
       <c r="B124" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C124" s="15"/>
       <c r="AD124" s="13"/>
@@ -3352,7 +3352,7 @@
     <row r="126" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="30"/>
       <c r="B126" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C126" s="15"/>
       <c r="AD126" s="13"/>
@@ -3370,7 +3370,7 @@
     <row r="128" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="30"/>
       <c r="B128" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C128" s="15"/>
       <c r="AD128" s="13"/>
@@ -3802,7 +3802,7 @@
         <v>31</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C159" s="15">
         <v>3</v>
@@ -3822,7 +3822,7 @@
     <row r="161" spans="1:32" s="16" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="30"/>
       <c r="B161" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C161" s="15"/>
       <c r="AD161" s="13"/>
@@ -3834,7 +3834,7 @@
         <v>1</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C162" s="15">
         <v>1</v>
@@ -3848,7 +3848,7 @@
         <v>2</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C163" s="15">
         <v>0.9</v>
@@ -3868,7 +3868,7 @@
     <row r="165" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="30"/>
       <c r="B165" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C165" s="15"/>
       <c r="AD165" s="13"/>
@@ -3922,7 +3922,7 @@
         <v>4</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C169" s="15">
         <v>1.2</v>
@@ -3942,7 +3942,7 @@
     <row r="171" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="30"/>
       <c r="B171" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C171" s="15"/>
       <c r="AD171" s="13"/>
@@ -3954,7 +3954,7 @@
         <v>1</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C172" s="18">
         <v>1</v>
@@ -3968,7 +3968,7 @@
         <v>2</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C173" s="18">
         <v>1</v>
@@ -3982,7 +3982,7 @@
         <v>3</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C174" s="18">
         <v>1</v>
@@ -3996,7 +3996,7 @@
         <v>4</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C175" s="18">
         <v>1</v>
@@ -4010,7 +4010,7 @@
         <v>5</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C176" s="18">
         <v>1</v>
@@ -4024,7 +4024,7 @@
         <v>6</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C177" s="18">
         <v>1</v>
@@ -4038,7 +4038,7 @@
         <v>7</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C178" s="18">
         <v>1</v>
@@ -4052,7 +4052,7 @@
         <v>8</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C179" s="18">
         <v>1</v>
@@ -4066,7 +4066,7 @@
         <v>9</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C180" s="18">
         <v>1</v>
@@ -4086,7 +4086,7 @@
     <row r="182" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="30"/>
       <c r="B182" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C182" s="15"/>
       <c r="AD182" s="13"/>
@@ -4350,7 +4350,7 @@
         <v>19</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C201" s="15">
         <v>0.8</v>
@@ -4370,7 +4370,7 @@
     <row r="203" spans="1:32" s="34" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="32"/>
       <c r="B203" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C203" s="28"/>
       <c r="AD203" s="35"/>
@@ -4388,7 +4388,7 @@
     <row r="205" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="30"/>
       <c r="B205" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C205" s="15"/>
       <c r="AD205" s="13"/>
@@ -4400,7 +4400,7 @@
         <v>1</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C206" s="15">
         <v>0.8</v>
@@ -4414,7 +4414,7 @@
         <v>2</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C207" s="15">
         <v>1</v>
@@ -4428,7 +4428,7 @@
         <v>3</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C208" s="15">
         <v>1.2</v>
@@ -4442,7 +4442,7 @@
         <v>4</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C209" s="15">
         <v>1.5</v>
@@ -4456,7 +4456,7 @@
         <v>5</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C210" s="15">
         <v>2</v>
@@ -4470,7 +4470,7 @@
         <v>6</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C211" s="15">
         <v>2.2000000000000002</v>
@@ -4484,7 +4484,7 @@
         <v>7</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C212" s="15">
         <v>2.5</v>
@@ -4498,7 +4498,7 @@
         <v>8</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C213" s="15">
         <v>3</v>
@@ -4530,7 +4530,7 @@
         <v>1</v>
       </c>
       <c r="B216" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C216" s="15"/>
       <c r="AD216" s="13"/>
@@ -4540,7 +4540,7 @@
     <row r="217" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A217" s="30"/>
       <c r="B217" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C217" s="18">
         <v>0.99</v>
@@ -4554,7 +4554,7 @@
         <v>2</v>
       </c>
       <c r="B218" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C218" s="18"/>
       <c r="AD218" s="13"/>
@@ -4564,7 +4564,7 @@
     <row r="219" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A219" s="30"/>
       <c r="B219" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C219" s="18">
         <v>0.99</v>
@@ -4578,7 +4578,7 @@
         <v>3</v>
       </c>
       <c r="B220" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C220" s="18"/>
       <c r="AD220" s="13"/>
@@ -4588,7 +4588,7 @@
     <row r="221" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A221" s="30"/>
       <c r="B221" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C221" s="18">
         <v>0.99</v>
@@ -4602,7 +4602,7 @@
         <v>4</v>
       </c>
       <c r="B222" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C222" s="18"/>
       <c r="AD222" s="13"/>
@@ -4612,7 +4612,7 @@
     <row r="223" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A223" s="30"/>
       <c r="B223" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C223" s="18">
         <v>0.98</v>
@@ -4626,7 +4626,7 @@
         <v>5</v>
       </c>
       <c r="B224" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C224" s="18"/>
       <c r="AD224" s="13"/>
@@ -4636,7 +4636,7 @@
     <row r="225" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A225" s="30"/>
       <c r="B225" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C225" s="18">
         <v>0.98</v>
@@ -4650,7 +4650,7 @@
         <v>6</v>
       </c>
       <c r="B226" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C226" s="18"/>
       <c r="AD226" s="13"/>
@@ -4660,7 +4660,7 @@
     <row r="227" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A227" s="30"/>
       <c r="B227" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C227" s="18">
         <v>0.99</v>
@@ -4719,13 +4719,13 @@
     </row>
     <row r="235" spans="1:32" ht="21" x14ac:dyDescent="0.25">
       <c r="B235" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="236" spans="1:32" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A236" s="30"/>
       <c r="B236" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C236" s="17">
         <v>80</v>
@@ -4737,7 +4737,7 @@
     <row r="237" spans="1:32" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A237" s="30"/>
       <c r="B237" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C237" s="17">
         <v>2</v>
@@ -4768,8 +4768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A299" workbookViewId="0">
-      <selection activeCell="D311" sqref="D311"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4800,7 +4800,7 @@
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" s="15"/>
     </row>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" s="15"/>
     </row>
@@ -5908,7 +5908,7 @@
         <v>100</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C106" s="19">
         <v>3</v>
@@ -5925,7 +5925,7 @@
     <row r="108" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="30"/>
       <c r="B108" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C108" s="15"/>
       <c r="AD108" s="13"/>
@@ -5965,7 +5965,7 @@
         <v>3</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>4</v>
+        <v>189</v>
       </c>
       <c r="C111" s="15">
         <v>2</v>
@@ -5979,7 +5979,7 @@
         <v>4</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C112" s="15">
         <v>2</v>
@@ -5993,7 +5993,7 @@
         <v>5</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C113" s="15">
         <v>2.2000000000000002</v>
@@ -6007,7 +6007,7 @@
         <v>6</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C114" s="15">
         <v>2.5</v>
@@ -6021,7 +6021,7 @@
         <v>7</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C115" s="15">
         <v>3</v>
@@ -6035,7 +6035,7 @@
         <v>8</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C116" s="15">
         <v>2</v>
@@ -6049,7 +6049,7 @@
         <v>9</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C117" s="15">
         <v>2</v>
@@ -6063,7 +6063,7 @@
         <v>10</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C118" s="15">
         <v>2</v>
@@ -6077,7 +6077,7 @@
         <v>11</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C119" s="15">
         <v>2</v>
@@ -6091,7 +6091,7 @@
         <v>12</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C120" s="15">
         <v>1.8</v>
@@ -6105,7 +6105,7 @@
         <v>13</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C121" s="15">
         <v>2.5</v>
@@ -6119,7 +6119,7 @@
         <v>14</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C122" s="15">
         <v>1.2</v>
@@ -6133,7 +6133,7 @@
         <v>15</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C123" s="15">
         <v>2.2000000000000002</v>
@@ -6147,7 +6147,7 @@
         <v>16</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C124" s="15">
         <v>1.5</v>
@@ -6161,7 +6161,7 @@
         <v>17</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C125" s="15">
         <v>1.8</v>
@@ -6175,7 +6175,7 @@
         <v>18</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C126" s="15">
         <v>2</v>
@@ -6189,7 +6189,7 @@
         <v>19</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C127" s="15">
         <v>3</v>
@@ -6203,7 +6203,7 @@
         <v>20</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C128" s="15">
         <v>3</v>
@@ -6217,7 +6217,7 @@
         <v>21</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C129" s="15">
         <v>1.5</v>
@@ -6231,7 +6231,7 @@
         <v>22</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C130" s="15">
         <v>2</v>
@@ -6245,7 +6245,7 @@
         <v>23</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C131" s="15">
         <v>2.5</v>
@@ -6259,7 +6259,7 @@
         <v>24</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C132" s="15">
         <v>2</v>
@@ -6273,7 +6273,7 @@
         <v>25</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C133" s="15">
         <v>2</v>
@@ -6287,7 +6287,7 @@
         <v>26</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C134" s="15">
         <v>2</v>
@@ -6301,7 +6301,7 @@
         <v>27</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C135" s="15">
         <v>1.5</v>
@@ -6315,7 +6315,7 @@
         <v>28</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C136" s="15">
         <v>3</v>
@@ -6329,7 +6329,7 @@
         <v>29</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C137" s="15">
         <v>2</v>
@@ -6343,7 +6343,7 @@
         <v>30</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C138" s="15">
         <v>2</v>
@@ -6357,7 +6357,7 @@
         <v>31</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C139" s="15">
         <v>2.5</v>
@@ -6371,7 +6371,7 @@
         <v>32</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C140" s="15">
         <v>2</v>
@@ -6385,7 +6385,7 @@
         <v>33</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C141" s="15">
         <v>2.5</v>
@@ -6399,7 +6399,7 @@
         <v>34</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C142" s="15">
         <v>2</v>
@@ -6413,7 +6413,7 @@
         <v>35</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C143" s="15">
         <v>2</v>
@@ -6427,7 +6427,7 @@
         <v>36</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C144" s="15">
         <v>2.5</v>
@@ -6441,7 +6441,7 @@
         <v>37</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C145" s="15">
         <v>2.2000000000000002</v>
@@ -6455,7 +6455,7 @@
         <v>38</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C146" s="15">
         <v>2.5</v>
@@ -6469,7 +6469,7 @@
         <v>39</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C147" s="15">
         <v>2</v>
@@ -6483,7 +6483,7 @@
         <v>40</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C148" s="15">
         <v>2</v>
@@ -6497,7 +6497,7 @@
         <v>41</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C149" s="15">
         <v>3</v>
@@ -6511,7 +6511,7 @@
         <v>42</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C150" s="15">
         <v>3</v>
@@ -6525,7 +6525,7 @@
         <v>43</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C151" s="15">
         <v>2</v>
@@ -6539,7 +6539,7 @@
         <v>44</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C152" s="15">
         <v>2.5</v>
@@ -6553,7 +6553,7 @@
         <v>45</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C153" s="15">
         <v>2.5</v>
@@ -6567,7 +6567,7 @@
         <v>46</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C154" s="15">
         <v>2</v>
@@ -6581,7 +6581,7 @@
         <v>47</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C155" s="15">
         <v>2</v>
@@ -6595,7 +6595,7 @@
         <v>48</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C156" s="15">
         <v>2.5</v>
@@ -6609,7 +6609,7 @@
         <v>49</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C157" s="15">
         <v>2.2999999999999998</v>
@@ -6623,7 +6623,7 @@
         <v>50</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C158" s="15">
         <v>2.2999999999999998</v>
@@ -6637,7 +6637,7 @@
         <v>51</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C159" s="15">
         <v>1.8</v>
@@ -6651,7 +6651,7 @@
         <v>52</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C160" s="15">
         <v>2</v>
@@ -6665,7 +6665,7 @@
         <v>53</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C161" s="15">
         <v>2.5</v>
@@ -6679,7 +6679,7 @@
         <v>54</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C162" s="15">
         <v>3</v>
@@ -6693,7 +6693,7 @@
         <v>55</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C163" s="15">
         <v>2</v>
@@ -6707,7 +6707,7 @@
         <v>56</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C164" s="15">
         <v>2.5</v>
@@ -6721,7 +6721,7 @@
         <v>57</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C165" s="15">
         <v>2</v>
@@ -6735,7 +6735,7 @@
         <v>58</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C166" s="15">
         <v>1.5</v>
@@ -6749,7 +6749,7 @@
         <v>59</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C167" s="15">
         <v>2</v>
@@ -6763,7 +6763,7 @@
         <v>60</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C168" s="15">
         <v>2</v>
@@ -6777,7 +6777,7 @@
         <v>61</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C169" s="15">
         <v>3</v>
@@ -6791,7 +6791,7 @@
         <v>62</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C170" s="15">
         <v>2.8</v>
@@ -6805,7 +6805,7 @@
         <v>63</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C171" s="15">
         <v>2.5</v>
@@ -6819,7 +6819,7 @@
         <v>64</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C172" s="15">
         <v>2</v>
@@ -6833,7 +6833,7 @@
         <v>65</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C173" s="15">
         <v>1.8</v>
@@ -6847,7 +6847,7 @@
         <v>66</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C174" s="15">
         <v>2</v>
@@ -6861,7 +6861,7 @@
         <v>67</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C175" s="15">
         <v>1.8</v>
@@ -6875,7 +6875,7 @@
         <v>68</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C176" s="15">
         <v>2.2000000000000002</v>
@@ -6889,7 +6889,7 @@
         <v>69</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C177" s="15">
         <v>1.5</v>
@@ -6903,7 +6903,7 @@
         <v>70</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C178" s="15">
         <v>2.5</v>
@@ -6917,7 +6917,7 @@
         <v>71</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C179" s="15">
         <v>1.8</v>
@@ -6931,7 +6931,7 @@
         <v>72</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C180" s="15">
         <v>2.5</v>
@@ -6945,7 +6945,7 @@
         <v>73</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C181" s="15">
         <v>2.2000000000000002</v>
@@ -6959,7 +6959,7 @@
         <v>74</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C182" s="15">
         <v>2.5</v>
@@ -6973,7 +6973,7 @@
         <v>75</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C183" s="15">
         <v>2.2000000000000002</v>
@@ -6987,7 +6987,7 @@
         <v>76</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C184" s="15">
         <v>3</v>
@@ -7001,7 +7001,7 @@
         <v>77</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C185" s="15">
         <v>2.8</v>
@@ -7015,7 +7015,7 @@
         <v>78</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C186" s="15">
         <v>2.5</v>
@@ -7029,7 +7029,7 @@
         <v>79</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C187" s="15">
         <v>2.2000000000000002</v>
@@ -7043,7 +7043,7 @@
         <v>80</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C188" s="15">
         <v>2</v>
@@ -7057,7 +7057,7 @@
         <v>81</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C189" s="15">
         <v>2</v>
@@ -7071,7 +7071,7 @@
         <v>82</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C190" s="15">
         <v>3</v>
@@ -7085,7 +7085,7 @@
         <v>83</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C191" s="15">
         <v>2.8</v>
@@ -7099,7 +7099,7 @@
         <v>84</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C192" s="15">
         <v>1.8</v>
@@ -7119,7 +7119,7 @@
     <row r="194" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="30"/>
       <c r="B194" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C194" s="15"/>
       <c r="AD194" s="13"/>
@@ -7137,7 +7137,7 @@
     <row r="196" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="30"/>
       <c r="B196" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C196" s="15"/>
       <c r="AD196" s="13"/>
@@ -7149,7 +7149,7 @@
         <v>1</v>
       </c>
       <c r="B197" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C197" s="18">
         <v>1.1000000000000001</v>
@@ -7163,7 +7163,7 @@
         <v>2</v>
       </c>
       <c r="B198" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C198" s="18">
         <v>1.1000000000000001</v>
@@ -7177,7 +7177,7 @@
         <v>3</v>
       </c>
       <c r="B199" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C199" s="18">
         <v>1.1000000000000001</v>
@@ -7191,7 +7191,7 @@
         <v>4</v>
       </c>
       <c r="B200" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C200" s="18">
         <v>1.1000000000000001</v>
@@ -7205,7 +7205,7 @@
         <v>5</v>
       </c>
       <c r="B201" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C201" s="18">
         <v>1.1000000000000001</v>
@@ -7219,7 +7219,7 @@
         <v>6</v>
       </c>
       <c r="B202" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C202" s="18">
         <v>1.1000000000000001</v>
@@ -7233,7 +7233,7 @@
         <v>7</v>
       </c>
       <c r="B203" s="27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C203" s="18">
         <v>1.1000000000000001</v>
@@ -7247,7 +7247,7 @@
         <v>8</v>
       </c>
       <c r="B204" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C204" s="18">
         <v>1.1000000000000001</v>
@@ -7261,7 +7261,7 @@
         <v>9</v>
       </c>
       <c r="B205" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C205" s="18">
         <v>1.1000000000000001</v>
@@ -7275,7 +7275,7 @@
         <v>10</v>
       </c>
       <c r="B206" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C206" s="18">
         <v>1.1000000000000001</v>
@@ -7289,7 +7289,7 @@
         <v>11</v>
       </c>
       <c r="B207" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C207" s="18">
         <v>1.1000000000000001</v>
@@ -7303,7 +7303,7 @@
         <v>12</v>
       </c>
       <c r="B208" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C208" s="18">
         <v>1.1000000000000001</v>
@@ -7317,7 +7317,7 @@
         <v>13</v>
       </c>
       <c r="B209" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C209" s="18">
         <v>1.1000000000000001</v>
@@ -7331,7 +7331,7 @@
         <v>14</v>
       </c>
       <c r="B210" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C210" s="18">
         <v>1.1000000000000001</v>
@@ -7345,7 +7345,7 @@
         <v>15</v>
       </c>
       <c r="B211" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C211" s="18">
         <v>1.1000000000000001</v>
@@ -7359,7 +7359,7 @@
         <v>16</v>
       </c>
       <c r="B212" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C212" s="18">
         <v>1.1000000000000001</v>
@@ -7373,7 +7373,7 @@
         <v>17</v>
       </c>
       <c r="B213" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C213" s="18">
         <v>1.1000000000000001</v>
@@ -7387,7 +7387,7 @@
         <v>18</v>
       </c>
       <c r="B214" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C214" s="18">
         <v>1.1000000000000001</v>
@@ -7401,7 +7401,7 @@
         <v>19</v>
       </c>
       <c r="B215" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C215" s="18">
         <v>1.1000000000000001</v>
@@ -7415,7 +7415,7 @@
         <v>20</v>
       </c>
       <c r="B216" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C216" s="18">
         <v>1.1000000000000001</v>
@@ -7429,7 +7429,7 @@
         <v>21</v>
       </c>
       <c r="B217" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C217" s="18">
         <v>1.1000000000000001</v>
@@ -7443,7 +7443,7 @@
         <v>22</v>
       </c>
       <c r="B218" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C218" s="18">
         <v>1.1000000000000001</v>
@@ -7457,7 +7457,7 @@
         <v>23</v>
       </c>
       <c r="B219" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C219" s="18">
         <v>1.1000000000000001</v>
@@ -7471,7 +7471,7 @@
         <v>24</v>
       </c>
       <c r="B220" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C220" s="18">
         <v>1.1000000000000001</v>
@@ -7491,7 +7491,7 @@
     <row r="222" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="30"/>
       <c r="B222" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C222" s="15"/>
       <c r="AD222" s="13"/>
@@ -7503,7 +7503,7 @@
         <v>1</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C223" s="15">
         <v>1</v>
@@ -7517,7 +7517,7 @@
         <v>2</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C224" s="15">
         <v>1</v>
@@ -7531,7 +7531,7 @@
         <v>3</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C225" s="15">
         <v>1</v>
@@ -7545,7 +7545,7 @@
         <v>4</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C226" s="15">
         <v>0.9</v>
@@ -7565,7 +7565,7 @@
     <row r="228" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="30"/>
       <c r="B228" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C228" s="15"/>
       <c r="AD228" s="13"/>
@@ -7583,7 +7583,7 @@
     <row r="230" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A230" s="30"/>
       <c r="B230" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C230" s="15"/>
       <c r="AD230" s="13"/>
@@ -7601,7 +7601,7 @@
     <row r="232" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A232" s="30"/>
       <c r="B232" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C232" s="15"/>
       <c r="AD232" s="13"/>
@@ -8033,7 +8033,7 @@
         <v>31</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C263" s="18">
         <v>1.1000000000000001</v>
@@ -8053,7 +8053,7 @@
     <row r="265" spans="1:32" s="16" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A265" s="30"/>
       <c r="B265" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C265" s="15"/>
       <c r="AD265" s="13"/>
@@ -8065,7 +8065,7 @@
         <v>1</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C266" s="15">
         <v>1</v>
@@ -8079,7 +8079,7 @@
         <v>2</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C267" s="28">
         <v>0.9</v>
@@ -8099,7 +8099,7 @@
     <row r="269" spans="1:32" s="16" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A269" s="30"/>
       <c r="B269" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C269" s="15"/>
       <c r="AD269" s="13"/>
@@ -8153,7 +8153,7 @@
         <v>4</v>
       </c>
       <c r="B273" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C273" s="18">
         <v>1.1000000000000001</v>
@@ -8173,7 +8173,7 @@
     <row r="275" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A275" s="30"/>
       <c r="B275" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C275" s="15"/>
       <c r="AD275" s="13"/>
@@ -8185,7 +8185,7 @@
         <v>1</v>
       </c>
       <c r="B276" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C276" s="18">
         <v>1</v>
@@ -8199,7 +8199,7 @@
         <v>2</v>
       </c>
       <c r="B277" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C277" s="18">
         <v>1</v>
@@ -8213,7 +8213,7 @@
         <v>3</v>
       </c>
       <c r="B278" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C278" s="18">
         <v>1</v>
@@ -8227,7 +8227,7 @@
         <v>4</v>
       </c>
       <c r="B279" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C279" s="18">
         <v>1</v>
@@ -8241,7 +8241,7 @@
         <v>5</v>
       </c>
       <c r="B280" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C280" s="18">
         <v>1</v>
@@ -8255,7 +8255,7 @@
         <v>6</v>
       </c>
       <c r="B281" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C281" s="18">
         <v>1</v>
@@ -8269,7 +8269,7 @@
         <v>7</v>
       </c>
       <c r="B282" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C282" s="18">
         <v>1</v>
@@ -8283,7 +8283,7 @@
         <v>8</v>
       </c>
       <c r="B283" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C283" s="18">
         <v>1</v>
@@ -8297,7 +8297,7 @@
         <v>9</v>
       </c>
       <c r="B284" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C284" s="18">
         <v>1</v>
@@ -8317,7 +8317,7 @@
     <row r="286" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A286" s="30"/>
       <c r="B286" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C286" s="15"/>
       <c r="AD286" s="13"/>
@@ -8581,7 +8581,7 @@
         <v>19</v>
       </c>
       <c r="B305" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C305" s="15">
         <v>0.8</v>
@@ -8601,7 +8601,7 @@
     <row r="307" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A307" s="30"/>
       <c r="B307" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C307" s="15"/>
       <c r="AD307" s="13"/>
@@ -8613,7 +8613,7 @@
         <v>1</v>
       </c>
       <c r="B308" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C308" s="15">
         <v>0.9</v>
@@ -8627,7 +8627,7 @@
         <v>2</v>
       </c>
       <c r="B309" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C309" s="15">
         <v>1.1000000000000001</v>
@@ -8641,7 +8641,7 @@
         <v>3</v>
       </c>
       <c r="B310" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C310" s="15">
         <v>1.2</v>
@@ -8661,7 +8661,7 @@
     <row r="312" spans="1:32" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A312" s="30"/>
       <c r="B312" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C312" s="15"/>
       <c r="AD312" s="13"/>
@@ -8673,7 +8673,7 @@
         <v>1</v>
       </c>
       <c r="B313" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C313" s="15">
         <v>0.8</v>
@@ -8687,7 +8687,7 @@
         <v>2</v>
       </c>
       <c r="B314" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C314" s="15">
         <v>1</v>
@@ -8701,7 +8701,7 @@
         <v>3</v>
       </c>
       <c r="B315" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C315" s="15">
         <v>1.2</v>
@@ -8715,7 +8715,7 @@
         <v>4</v>
       </c>
       <c r="B316" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C316" s="15">
         <v>1.5</v>
@@ -8729,7 +8729,7 @@
         <v>5</v>
       </c>
       <c r="B317" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C317" s="15">
         <v>2</v>
@@ -8743,7 +8743,7 @@
         <v>6</v>
       </c>
       <c r="B318" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C318" s="15">
         <v>2.2000000000000002</v>
@@ -8757,7 +8757,7 @@
         <v>7</v>
       </c>
       <c r="B319" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C319" s="15">
         <v>2.5</v>
@@ -8771,7 +8771,7 @@
         <v>8</v>
       </c>
       <c r="B320" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C320" s="15">
         <v>3</v>
@@ -8803,7 +8803,7 @@
         <v>1</v>
       </c>
       <c r="B323" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C323" s="15"/>
       <c r="AD323" s="13"/>
@@ -8813,7 +8813,7 @@
     <row r="324" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A324" s="30"/>
       <c r="B324" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C324" s="18">
         <v>0.99</v>
@@ -8827,7 +8827,7 @@
         <v>2</v>
       </c>
       <c r="B325" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C325" s="18"/>
       <c r="AD325" s="13"/>
@@ -8837,7 +8837,7 @@
     <row r="326" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A326" s="30"/>
       <c r="B326" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C326" s="18">
         <v>0.99</v>
@@ -8851,7 +8851,7 @@
         <v>3</v>
       </c>
       <c r="B327" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C327" s="18"/>
       <c r="AD327" s="13"/>
@@ -8861,7 +8861,7 @@
     <row r="328" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A328" s="30"/>
       <c r="B328" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C328" s="18">
         <v>0.99</v>
@@ -8875,7 +8875,7 @@
         <v>4</v>
       </c>
       <c r="B329" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C329" s="18"/>
       <c r="AD329" s="13"/>
@@ -8885,7 +8885,7 @@
     <row r="330" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A330" s="30"/>
       <c r="B330" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C330" s="18">
         <v>0.98</v>
@@ -8899,7 +8899,7 @@
         <v>5</v>
       </c>
       <c r="B331" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C331" s="18"/>
       <c r="AD331" s="13"/>
@@ -8909,7 +8909,7 @@
     <row r="332" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A332" s="30"/>
       <c r="B332" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C332" s="18">
         <v>0.98</v>
@@ -8923,7 +8923,7 @@
         <v>6</v>
       </c>
       <c r="B333" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C333" s="18"/>
       <c r="AD333" s="13"/>
@@ -8933,7 +8933,7 @@
     <row r="334" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A334" s="30"/>
       <c r="B334" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C334" s="18">
         <v>0.99</v>
@@ -8992,13 +8992,13 @@
     </row>
     <row r="342" spans="1:32" ht="21" x14ac:dyDescent="0.25">
       <c r="B342" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="343" spans="1:32" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A343" s="30"/>
       <c r="B343" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C343" s="17">
         <v>80</v>
@@ -9010,7 +9010,7 @@
     <row r="344" spans="1:32" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A344" s="30"/>
       <c r="B344" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C344" s="17">
         <v>2</v>

</xml_diff>